<commit_message>
Completed remove_whitespace script in jupyter
Still getting odd unicode characters; I think it's because of MS Word
</commit_message>
<xml_diff>
--- a/Engine_5/vets_test.xlsx
+++ b/Engine_5/vets_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mo/Documents/Warren Fire/Engine 5/War_Vets/Engine_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05794613-3FBB-264C-AD43-5C4887D35059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DB87BA-AD2B-5049-B158-037D7ABE839A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{3911A830-49ED-654D-A5B2-8B47467BD25A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="147">
   <si>
     <t>Last Name</t>
   </si>
@@ -407,9 +407,6 @@
     <t>WUJICK</t>
   </si>
   <si>
-    <t xml:space="preserve"> EDWARD W</t>
-  </si>
-  <si>
     <t>WW2</t>
   </si>
   <si>
@@ -465,6 +462,18 @@
   </si>
   <si>
     <t>EDWARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  THEODORE W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARTEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EDWARD W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CAMARA</t>
   </si>
 </sst>
 </file>
@@ -818,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF5BF59-53AD-2647-8506-1E55C8B4552C}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1641,7 +1650,7 @@
         <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -1722,7 +1731,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="B65" t="s">
         <v>111</v>
@@ -1851,13 +1860,13 @@
         <v>123</v>
       </c>
       <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
         <v>124</v>
-      </c>
-      <c r="C74" t="b">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1871,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1879,139 +1888,139 @@
         <v>123</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" t="s">
         <v>127</v>
       </c>
-      <c r="B77" t="s">
-        <v>128</v>
-      </c>
       <c r="C77" t="b">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
         <v>130</v>
-      </c>
-      <c r="B79" t="s">
-        <v>143</v>
-      </c>
-      <c r="C79" t="b">
-        <v>0</v>
-      </c>
-      <c r="D79" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" t="s">
         <v>130</v>
-      </c>
-      <c r="B80" t="s">
-        <v>132</v>
-      </c>
-      <c r="C80" t="b">
-        <v>0</v>
-      </c>
-      <c r="D80" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>132</v>
+      </c>
+      <c r="B81" t="s">
         <v>133</v>
       </c>
-      <c r="B81" t="s">
-        <v>134</v>
-      </c>
       <c r="C81" t="b">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>134</v>
+      </c>
+      <c r="B82" t="s">
         <v>135</v>
       </c>
-      <c r="B82" t="s">
-        <v>136</v>
-      </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" t="s">
         <v>137</v>
       </c>
-      <c r="B83" t="s">
-        <v>138</v>
-      </c>
       <c r="C83" t="b">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>138</v>
+      </c>
+      <c r="B84" t="s">
         <v>139</v>
       </c>
-      <c r="B84" t="s">
-        <v>140</v>
-      </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" t="s">
         <v>141</v>
       </c>
-      <c r="B85" t="s">
-        <v>142</v>
-      </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save point for adding to compare script
</commit_message>
<xml_diff>
--- a/Engine_5/vets_test.xlsx
+++ b/Engine_5/vets_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mo/Documents/Warren Fire/Engine 5/War_Vets/Engine_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DB87BA-AD2B-5049-B158-037D7ABE839A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DD7DF-FD60-D549-839C-0729C67C0502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{3911A830-49ED-654D-A5B2-8B47467BD25A}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>WW1</t>
   </si>
   <si>
-    <t>ACKERMAN</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SAMUEL</t>
   </si>
   <si>
@@ -474,6 +471,9 @@
   </si>
   <si>
     <t xml:space="preserve"> CAMARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ACKERMAN</t>
   </si>
 </sst>
 </file>
@@ -827,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF5BF59-53AD-2647-8506-1E55C8B4552C}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,10 +863,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -877,10 +877,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -891,10 +891,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -905,10 +905,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -961,10 +961,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -975,10 +975,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
         <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1171,10 +1171,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
         <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1199,10 +1199,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
         <v>44</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
         <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
         <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
         <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -1269,758 +1269,758 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
       <c r="C32" t="b">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
         <v>63</v>
       </c>
-      <c r="B38" t="s">
-        <v>64</v>
-      </c>
       <c r="C38" t="b">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
         <v>65</v>
       </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
         <v>67</v>
       </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
       <c r="C40" t="b">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
         <v>70</v>
       </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
       <c r="C43" t="b">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" t="s">
         <v>74</v>
       </c>
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
       <c r="C44" t="b">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
         <v>77</v>
       </c>
-      <c r="B46" t="s">
-        <v>78</v>
-      </c>
       <c r="C46" t="b">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
         <v>80</v>
       </c>
-      <c r="B48" t="s">
-        <v>81</v>
-      </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" t="s">
         <v>82</v>
       </c>
-      <c r="B49" t="s">
-        <v>83</v>
-      </c>
       <c r="C49" t="b">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
         <v>84</v>
       </c>
-      <c r="B50" t="s">
-        <v>85</v>
-      </c>
       <c r="C50" t="b">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
         <v>86</v>
       </c>
-      <c r="B51" t="s">
-        <v>87</v>
-      </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" t="s">
         <v>89</v>
       </c>
-      <c r="B53" t="s">
-        <v>90</v>
-      </c>
       <c r="C53" t="b">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
         <v>91</v>
       </c>
-      <c r="B54" t="s">
-        <v>92</v>
-      </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" t="s">
         <v>93</v>
       </c>
-      <c r="B55" t="s">
-        <v>94</v>
-      </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" t="s">
         <v>95</v>
       </c>
-      <c r="B56" t="s">
-        <v>96</v>
-      </c>
       <c r="C56" t="b">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" t="s">
         <v>97</v>
       </c>
-      <c r="B57" t="s">
-        <v>98</v>
-      </c>
       <c r="C57" t="b">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" t="s">
         <v>99</v>
       </c>
-      <c r="B58" t="s">
-        <v>100</v>
-      </c>
       <c r="C58" t="b">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" t="s">
         <v>101</v>
       </c>
-      <c r="B60" t="s">
-        <v>102</v>
-      </c>
       <c r="C60" t="b">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" t="s">
         <v>103</v>
       </c>
-      <c r="B61" t="s">
-        <v>104</v>
-      </c>
       <c r="C61" t="b">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" t="s">
         <v>105</v>
       </c>
-      <c r="B62" t="s">
-        <v>106</v>
-      </c>
       <c r="C62" t="b">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
         <v>107</v>
       </c>
-      <c r="B63" t="s">
-        <v>108</v>
-      </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" t="s">
         <v>114</v>
       </c>
-      <c r="B68" t="s">
-        <v>115</v>
-      </c>
       <c r="C68" t="b">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" t="s">
         <v>116</v>
       </c>
-      <c r="B69" t="s">
-        <v>117</v>
-      </c>
       <c r="C69" t="b">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" t="s">
         <v>120</v>
       </c>
-      <c r="B72" t="s">
-        <v>121</v>
-      </c>
       <c r="C72" t="b">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
         <v>123</v>
-      </c>
-      <c r="B74" t="s">
-        <v>145</v>
-      </c>
-      <c r="C74" t="b">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
         <v>123</v>
-      </c>
-      <c r="B75" t="s">
-        <v>45</v>
-      </c>
-      <c r="C75" t="b">
-        <v>0</v>
-      </c>
-      <c r="D75" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
         <v>123</v>
-      </c>
-      <c r="B76" t="s">
-        <v>125</v>
-      </c>
-      <c r="C76" t="b">
-        <v>0</v>
-      </c>
-      <c r="D76" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" t="s">
         <v>126</v>
       </c>
-      <c r="B77" t="s">
-        <v>127</v>
-      </c>
       <c r="C77" t="b">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" t="s">
         <v>129</v>
-      </c>
-      <c r="B80" t="s">
-        <v>131</v>
-      </c>
-      <c r="C80" t="b">
-        <v>0</v>
-      </c>
-      <c r="D80" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" t="s">
         <v>132</v>
       </c>
-      <c r="B81" t="s">
-        <v>133</v>
-      </c>
       <c r="C81" t="b">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>133</v>
+      </c>
+      <c r="B82" t="s">
         <v>134</v>
       </c>
-      <c r="B82" t="s">
-        <v>135</v>
-      </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" t="s">
         <v>136</v>
       </c>
-      <c r="B83" t="s">
-        <v>137</v>
-      </c>
       <c r="C83" t="b">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" t="s">
         <v>138</v>
       </c>
-      <c r="B84" t="s">
-        <v>139</v>
-      </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" t="s">
         <v>140</v>
       </c>
-      <c r="B85" t="s">
-        <v>141</v>
-      </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>